<commit_message>
working on conversion check, WIP ClinVar - MedGen identifiers = findings -> check DODO
</commit_message>
<xml_diff>
--- a/inst/documentation/CrossreferencesEdges.xlsx
+++ b/inst/documentation/CrossreferencesEdges.xlsx
@@ -5,16 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\RD\Informatics\TPI\Data science\R-Packages\DODO\build\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\RD\Informatics\TPI\Data science\R-Packages\DODO\inst\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6D06FF-CB7A-43C2-86C8-640F2365D20D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4C877C-3F40-4BDA-B2F9-20C24E77975E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{37D872A3-D4AA-42BA-9B9E-34DA1B138CC7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12380" activeTab="1" xr2:uid="{37D872A3-D4AA-42BA-9B9E-34DA1B138CC7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Default_xref_edges" sheetId="1" r:id="rId1"/>
+    <sheet name="Max_ambiguity_3_across_DBs" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$B$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="21">
   <si>
     <t>DB2</t>
   </si>
@@ -66,6 +71,33 @@
   </si>
   <si>
     <t xml:space="preserve">MONDO </t>
+  </si>
+  <si>
+    <t>OMIM</t>
+  </si>
+  <si>
+    <t>Cortellis_condition</t>
+  </si>
+  <si>
+    <t>Cortellis_indication</t>
+  </si>
+  <si>
+    <t>ClinVar</t>
+  </si>
+  <si>
+    <t>SNOMEDCT</t>
+  </si>
+  <si>
+    <t>GARD</t>
+  </si>
+  <si>
+    <t>NCIt</t>
+  </si>
+  <si>
+    <t>MetaBase_disease</t>
+  </si>
+  <si>
+    <t>MEDDRA</t>
   </si>
 </sst>
 </file>
@@ -428,13 +460,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7989604F-B1F2-44C9-A03F-056964347B1D}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -442,7 +474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -450,7 +482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -458,7 +490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -466,7 +498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -474,7 +506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -482,7 +514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -490,7 +522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -498,7 +530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -506,7 +538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -514,7 +546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -522,7 +554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -530,7 +562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -545,4 +577,537 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F80E06-465D-4935-8F64-5C18C90B3CA9}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6328125" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C5B8F6-606A-4BEF-803E-37AD57117CD5}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add type to disNet and to show_relations
</commit_message>
<xml_diff>
--- a/inst/documentation/CrossreferencesEdges.xlsx
+++ b/inst/documentation/CrossreferencesEdges.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\RD\Informatics\TPI\Data science\R-Packages\DODO\inst\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4C877C-3F40-4BDA-B2F9-20C24E77975E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815FDB40-9A7D-4AEF-A20F-5451EE301226}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12380" activeTab="1" xr2:uid="{37D872A3-D4AA-42BA-9B9E-34DA1B138CC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Default_xref_edges" sheetId="1" r:id="rId1"/>
-    <sheet name="Max_ambiguity_3_across_DBs" sheetId="2" r:id="rId2"/>
+    <sheet name="Max_ambiguity_4_across_DBs" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -584,7 +584,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B31"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updating database: adding mesh, omim, orphanet to is_xref, making get_related  symmetric, correcting FA edge from nba edges
</commit_message>
<xml_diff>
--- a/inst/documentation/CrossreferencesEdges.xlsx
+++ b/inst/documentation/CrossreferencesEdges.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\RD\Informatics\TPI\Data science\R-Packages\DODO\inst\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U060109.UCB-CORP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815FDB40-9A7D-4AEF-A20F-5451EE301226}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A07B645-0ED8-43E5-98AA-3FA011DEF90B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12380" activeTab="1" xr2:uid="{37D872A3-D4AA-42BA-9B9E-34DA1B138CC7}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Max_ambiguity_4_across_DBs!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="22">
   <si>
     <t>DB2</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>MEDDRA</t>
+  </si>
+  <si>
+    <t>OPRHA</t>
   </si>
 </sst>
 </file>
@@ -581,10 +584,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F80E06-465D-4935-8F64-5C18C90B3CA9}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,26 +608,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -632,15 +635,15 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -648,7 +651,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -656,7 +659,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -664,15 +667,15 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -680,12 +683,12 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
@@ -693,39 +696,39 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -733,39 +736,39 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -773,34 +776,34 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -808,42 +811,191 @@
         <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B1" xr:uid="{72059B75-4B77-4330-8381-982D7621E2EE}">
+    <sortState ref="A2:B49">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>